<commit_message>
Reordering heatbed components in BOM
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 3D 400 BOM.xlsx
+++ b/BOM/V-King PRO 3D 400 BOM.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="530" documentId="11_C72AD000C5F844E0111E73BF19DBFC71502D2EF0" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{5E68F9EE-2F15-4965-9E9D-A10786D9200D}"/>
+  <xr:revisionPtr revIDLastSave="555" documentId="11_C72AD000C5F844E0111E73BF19DBFC71502D2EF0" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{22BF3F69-38AC-4792-80AF-D4DF29FBDE48}"/>
   <bookViews>
-    <workbookView xWindow="1176" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2112" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$1:$K$119</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$1:$K$122</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
@@ -25,14 +25,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{72F1B1DD-E67E-4287-9722-7C91C5A7BE2C}" keepAlive="1" name="Query - Table1" description="Connection to the 'Table1' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Query - Table1" description="Connection to the 'Table1' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Table1;Extended Properties=&quot;&quot;" command="SELECT * FROM [Table1]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="366">
   <si>
     <t>Part Name</t>
   </si>
@@ -1060,9 +1060,6 @@
     <t>Controller case parts</t>
   </si>
   <si>
-    <t>Ekstra print parts for this config</t>
-  </si>
-  <si>
     <t>Mechatronical components</t>
   </si>
   <si>
@@ -1121,6 +1118,18 @@
   </si>
   <si>
     <t>Belt lock Upper</t>
+  </si>
+  <si>
+    <t>These are cabinet print parts for this config</t>
+  </si>
+  <si>
+    <t>PSU Case</t>
+  </si>
+  <si>
+    <t>PSU Lid</t>
+  </si>
+  <si>
+    <t>Heatbed components</t>
   </si>
 </sst>
 </file>
@@ -1245,19 +1254,19 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_([$EUR]\ * #,##0.00_);_([$EUR]\ * \(#,##0.00\);_([$EUR]\ * &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="_([$EUR]\ * #,##0.00_);_([$EUR]\ * \(#,##0.00\);_([$EUR]\ * &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="_([$EUR]\ * #,##0.00_);_([$EUR]\ * \(#,##0.00\);_([$EUR]\ * &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1285,7 +1294,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{D19F3DE5-56AE-43A6-BF8C-216C35D573E1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="14">
     <queryTableFields count="11">
       <queryTableField id="1" name="Part Name" tableColumnId="1"/>
@@ -1308,26 +1317,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9F76A420-7539-4EA8-B971-D3C24F0FF152}" name="Table1_2" displayName="Table1_2" ref="A1:K120" tableType="queryTable" totalsRowCount="1">
-  <autoFilter ref="A1:K119" xr:uid="{D9DBC87E-E3EB-4128-B66B-0280679601F7}"/>
-  <sortState ref="A2:K119">
-    <sortCondition ref="K1:K119"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9F76A420-7539-4EA8-B971-D3C24F0FF152}" name="Table1_2" displayName="Table1_2" ref="A1:K123" tableType="queryTable" totalsRowCount="1">
+  <autoFilter ref="A1:K122" xr:uid="{D9DBC87E-E3EB-4128-B66B-0280679601F7}"/>
+  <sortState ref="A2:K122">
+    <sortCondition ref="K1:K122"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{AD105796-BC3D-4F71-8012-D88AD4FD6233}" uniqueName="1" name="Part Name" queryTableFieldId="1" dataDxfId="15"/>
     <tableColumn id="3" xr3:uid="{9B940B3B-13CE-4EFA-BAF5-8030A677FF27}" uniqueName="3" name="Part Number" queryTableFieldId="3" dataDxfId="14" totalsRowDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00DE9FC5-CAF4-44E4-B99B-6ADF6EB252D1}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{778813CF-2179-4099-B9EA-71162D34F4A2}" uniqueName="5" name="Make/Buy" queryTableFieldId="5" dataDxfId="13" totalsRowDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00DE9FC5-CAF4-44E4-B99B-6ADF6EB252D1}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{778813CF-2179-4099-B9EA-71162D34F4A2}" uniqueName="5" name="Make/Buy" queryTableFieldId="5" dataDxfId="12" totalsRowDxfId="5"/>
     <tableColumn id="6" xr3:uid="{D9CDA1E5-D138-4A55-8901-A09B00188167}" uniqueName="6" name="Quantity" queryTableFieldId="6"/>
     <tableColumn id="7" xr3:uid="{FFCE91F0-00D6-4E2D-AA7F-E01B191EAA59}" uniqueName="7" name="Order Quantity" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{6D94E448-3558-4A45-A375-23F2CA012E0F}" uniqueName="8" name="Material" queryTableFieldId="8" dataDxfId="12" totalsRowDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{493843DC-3B43-440E-9737-42338786D57E}" uniqueName="9" name="Mass" queryTableFieldId="9" dataDxfId="11" totalsRowDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{F4486787-27B4-4A40-A2E5-26D8FF459FBB}" uniqueName="10" name="Item Price" totalsRowLabel="Part filament approximation" queryTableFieldId="10" dataDxfId="7" totalsRowDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{09B941BA-A840-42C2-907C-15716549B38B}" uniqueName="12" name="Row Price" totalsRowFunction="custom" queryTableFieldId="13" dataDxfId="10" totalsRowDxfId="1">
+    <tableColumn id="8" xr3:uid="{6D94E448-3558-4A45-A375-23F2CA012E0F}" uniqueName="8" name="Material" queryTableFieldId="8" dataDxfId="11" totalsRowDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{493843DC-3B43-440E-9737-42338786D57E}" uniqueName="9" name="Mass" queryTableFieldId="9" dataDxfId="10" totalsRowDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{F4486787-27B4-4A40-A2E5-26D8FF459FBB}" uniqueName="10" name="Item Price" totalsRowLabel="Part filament approximation" queryTableFieldId="10" dataDxfId="9" totalsRowDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{09B941BA-A840-42C2-907C-15716549B38B}" uniqueName="12" name="Row Price" totalsRowFunction="custom" queryTableFieldId="13" dataDxfId="8" totalsRowDxfId="1">
       <calculatedColumnFormula>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</calculatedColumnFormula>
-      <totalsRowFormula>SUBTOTAL(109,J84:J119)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,J87:J122)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{FF512CFE-168A-4A3A-9427-353A988F7E08}" uniqueName="11" name="Category" queryTableFieldId="11" dataDxfId="9" totalsRowDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{FF512CFE-168A-4A3A-9427-353A988F7E08}" uniqueName="11" name="Category" queryTableFieldId="11" dataDxfId="7" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1674,7 +1683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D96BDA-DD41-4F1E-950D-DAA22706FDDE}">
-  <dimension ref="A1:K122"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1740,7 +1752,7 @@
         <v>341</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>342</v>
+        <v>362</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="3"/>
@@ -1754,7 +1766,9 @@
       <c r="B4" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>363</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>41</v>
       </c>
@@ -1826,7 +1840,9 @@
       <c r="B6" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>364</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>41</v>
       </c>
@@ -2037,7 +2053,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="10" t="s">
@@ -2067,7 +2083,7 @@
         <v>340</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2115,13 +2131,13 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>206</v>
+        <v>146</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>18</v>
@@ -2136,7 +2152,7 @@
         <v>316</v>
       </c>
       <c r="H16" s="2">
-        <v>0.40181027259318802</v>
+        <v>5.5130859982009299E-3</v>
       </c>
       <c r="I16" s="3">
         <v>40</v>
@@ -2151,13 +2167,13 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>146</v>
+        <v>262</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>146</v>
+        <v>262</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>18</v>
@@ -2172,14 +2188,14 @@
         <v>316</v>
       </c>
       <c r="H17" s="2">
-        <v>5.5130859982009299E-3</v>
+        <v>2.1882012078843299E-2</v>
       </c>
       <c r="I17" s="3">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J17" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>175</v>
@@ -2187,13 +2203,13 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>262</v>
+        <v>328</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>262</v>
+        <v>328</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>18</v>
@@ -2208,14 +2224,14 @@
         <v>316</v>
       </c>
       <c r="H18" s="2">
-        <v>2.1882012078843299E-2</v>
+        <v>0.22522779179250799</v>
       </c>
       <c r="I18" s="3">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J18" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>175</v>
@@ -2223,13 +2239,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>325</v>
+        <v>279</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>18</v>
@@ -2244,14 +2260,14 @@
         <v>316</v>
       </c>
       <c r="H19" s="2">
-        <v>0.22522779179250799</v>
+        <v>0.102542513772092</v>
       </c>
       <c r="I19" s="3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="J19" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>175</v>
@@ -2259,13 +2275,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>279</v>
+        <v>184</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>280</v>
+        <v>185</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>329</v>
+        <v>185</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>18</v>
@@ -2280,14 +2296,14 @@
         <v>316</v>
       </c>
       <c r="H20" s="2">
-        <v>0.102542513772092</v>
+        <v>1.09976688532335E-2</v>
       </c>
       <c r="I20" s="3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J20" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>175</v>
@@ -2295,13 +2311,13 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>184</v>
+        <v>297</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>185</v>
+        <v>298</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>185</v>
+        <v>331</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>18</v>
@@ -2316,14 +2332,14 @@
         <v>316</v>
       </c>
       <c r="H21" s="2">
-        <v>1.09976688532335E-2</v>
+        <v>6.0324503930431601E-2</v>
       </c>
       <c r="I21" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J21" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>175</v>
@@ -2331,13 +2347,13 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>18</v>
@@ -2352,14 +2368,14 @@
         <v>316</v>
       </c>
       <c r="H22" s="2">
-        <v>0.146734344823789</v>
+        <v>0.137965563144898</v>
       </c>
       <c r="I22" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J22" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>175</v>
@@ -2367,35 +2383,35 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>297</v>
+        <v>269</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>298</v>
+        <v>270</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>316</v>
       </c>
       <c r="H23" s="2">
-        <v>6.0324503930431601E-2</v>
+        <v>1.6605292973304899E-2</v>
       </c>
       <c r="I23" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J23" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>175</v>
@@ -2403,13 +2419,13 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>299</v>
+        <v>345</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>300</v>
+        <v>345</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>18</v>
@@ -2424,14 +2440,14 @@
         <v>316</v>
       </c>
       <c r="H24" s="2">
-        <v>0.137965563144898</v>
+        <v>5.3667075047124403E-3</v>
       </c>
       <c r="I24" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J24" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>175</v>
@@ -2439,13 +2455,13 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>269</v>
+        <v>76</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>270</v>
+        <v>77</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>18</v>
@@ -2460,132 +2476,109 @@
         <v>316</v>
       </c>
       <c r="H25" s="2">
-        <v>1.6605292973304899E-2</v>
+        <v>2.0129610048330898E-3</v>
       </c>
       <c r="I25" s="3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J25" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="H26" s="2">
-        <v>5.3667075047124403E-3</v>
-      </c>
-      <c r="I26" s="3">
-        <v>1</v>
-      </c>
-      <c r="J26" s="3">
-        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>1</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>175</v>
-      </c>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="H26" s="8"/>
+      <c r="I26" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="J26" s="5">
+        <f>SUBTOTAL(109,J15:J25)</f>
+        <v>205</v>
+      </c>
+      <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-      <c r="F27">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="H27" s="2">
-        <v>2.0129610048330898E-3</v>
-      </c>
-      <c r="I27" s="3">
-        <v>2</v>
-      </c>
-      <c r="J27" s="3">
-        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>4</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>175</v>
-      </c>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="6"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="9" t="s">
-        <v>344</v>
-      </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="J28" s="5">
-        <f>SUBTOTAL(109,J15:J27)</f>
-        <v>250</v>
-      </c>
-      <c r="K28" s="6"/>
+      <c r="A28" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1.3933091100481101</v>
+      </c>
+      <c r="I29" s="3">
+        <v>30</v>
+      </c>
+      <c r="J29" s="3">
+        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
+        <v>30</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>143</v>
+        <v>290</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>144</v>
+        <v>291</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>18</v>
@@ -2597,17 +2590,17 @@
         <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H30" s="2">
-        <v>3.7725910242318597E-2</v>
+        <v>0.146734344823789</v>
       </c>
       <c r="I30" s="3">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="J30" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>175</v>
@@ -2615,13 +2608,13 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>174</v>
+        <v>322</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>174</v>
+        <v>205</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>336</v>
+        <v>206</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>18</v>
@@ -2633,17 +2626,17 @@
         <v>1</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H31" s="2">
-        <v>1.6886056678943599E-2</v>
+        <v>0.40181027259318802</v>
       </c>
       <c r="I31" s="3">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="J31" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>175</v>
@@ -2651,13 +2644,13 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>313</v>
+        <v>209</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>313</v>
+        <v>209</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>314</v>
+        <v>210</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>18</v>
@@ -2669,103 +2662,62 @@
         <v>1</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>318</v>
+        <v>19</v>
       </c>
       <c r="H32" s="2">
-        <v>3.9148590193938501E-2</v>
+        <v>2.5919999999999899</v>
       </c>
       <c r="I32" s="3">
+        <v>55</v>
+      </c>
+      <c r="J32" s="3">
+        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
+        <v>55</v>
+      </c>
+      <c r="K32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="3">
-        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>20</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33">
-        <v>4</v>
-      </c>
-      <c r="F33">
-        <v>4</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="H33" s="2">
-        <v>0.54644527252961195</v>
-      </c>
-      <c r="I33" s="3">
-        <v>10</v>
-      </c>
-      <c r="J33" s="3">
-        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>40</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>175</v>
-      </c>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="H33" s="8"/>
+      <c r="I33" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="J33" s="5">
+        <f>SUBTOTAL(109,J29:J32)</f>
+        <v>130</v>
+      </c>
+      <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34">
-        <v>10</v>
-      </c>
-      <c r="F34">
-        <v>10</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="H34" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="I34" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="J34" s="3">
-        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>35</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>175</v>
-      </c>
+      <c r="A34" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="1"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>179</v>
+        <v>143</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>18</v>
@@ -2780,14 +2732,14 @@
         <v>318</v>
       </c>
       <c r="H35" s="2">
-        <v>1.0838154518140099E-2</v>
+        <v>3.7725910242318597E-2</v>
       </c>
       <c r="I35" s="3">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="J35" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>175</v>
@@ -2795,35 +2747,35 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>57</v>
+        <v>174</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>58</v>
+        <v>174</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E36">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F36">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>318</v>
       </c>
       <c r="H36" s="2">
-        <v>5.6951527903449503E-3</v>
+        <v>1.6886056678943599E-2</v>
       </c>
       <c r="I36" s="3">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="J36" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>175</v>
@@ -2831,35 +2783,35 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>113</v>
+        <v>313</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>115</v>
+        <v>314</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E37">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F37">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>318</v>
       </c>
       <c r="H37" s="2">
-        <v>2.6839940507117702E-3</v>
+        <v>3.9148590193938501E-2</v>
       </c>
       <c r="I37" s="3">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="J37" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>175</v>
@@ -2867,275 +2819,281 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E38">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F38">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>318</v>
       </c>
       <c r="H38" s="2">
-        <v>2.60154274818712E-3</v>
+        <v>0.54644527252961195</v>
       </c>
       <c r="I38" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J38" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="9" t="s">
-        <v>344</v>
-      </c>
-      <c r="H39" s="8"/>
-      <c r="I39" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="J39" s="5">
-        <f>SUBTOTAL(109,J30:J38)</f>
-        <v>285</v>
-      </c>
-      <c r="K39" s="6"/>
+      <c r="A39" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39">
+        <v>10</v>
+      </c>
+      <c r="F39">
+        <v>10</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="I39" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="J39" s="3">
+        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
+        <v>35</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
-        <v>347</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="H40" s="2">
+        <v>1.0838154518140099E-2</v>
+      </c>
+      <c r="I40" s="3">
+        <v>10</v>
+      </c>
+      <c r="J40" s="3">
+        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
+        <v>10</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>337</v>
+      </c>
       <c r="D41" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E41">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="F41">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>71</v>
+        <v>318</v>
       </c>
       <c r="H41" s="2">
-        <v>2.36974260851105E-4</v>
+        <v>5.6951527903449503E-3</v>
       </c>
       <c r="I41" s="3">
-        <v>0.1</v>
+        <v>4</v>
       </c>
       <c r="J41" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>7.7</v>
+        <v>16</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>33</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>235</v>
+        <v>113</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C42" s="1"/>
+        <v>309</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="D42" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E42">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F42">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>26</v>
+        <v>318</v>
       </c>
       <c r="H42" s="2">
-        <v>6.5170950498219301E-3</v>
+        <v>2.6839940507117702E-3</v>
       </c>
       <c r="I42" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J42" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>33</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E43">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="F43">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>26</v>
+        <v>318</v>
       </c>
       <c r="H43" s="2">
-        <v>1.9298375811925401E-3</v>
+        <v>2.60154274818712E-3</v>
       </c>
       <c r="I43" s="3">
-        <v>0.2</v>
+        <v>3</v>
       </c>
       <c r="J43" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>6.8000000000000007</v>
+        <v>24</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>33</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E44">
-        <v>12</v>
-      </c>
-      <c r="F44">
-        <v>12</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H44" s="2">
-        <v>1.8554944377140699E-3</v>
-      </c>
-      <c r="I44" s="3">
-        <v>0.13</v>
-      </c>
-      <c r="J44" s="3">
-        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>1.56</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="H44" s="8"/>
+      <c r="I44" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="J44" s="5">
+        <f>SUBTOTAL(109,J35:J43)</f>
+        <v>285</v>
+      </c>
+      <c r="K44" s="6"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="A45" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E45">
-        <v>4</v>
-      </c>
-      <c r="F45">
-        <v>4</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H45" s="2">
-        <v>6.5954579555748804E-3</v>
-      </c>
-      <c r="I45" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="J45" s="3">
-        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.4</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="D45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="1"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E46">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="F46">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="H46" s="2">
-        <v>5.8288025643596902E-3</v>
+        <v>2.36974260851105E-4</v>
       </c>
       <c r="I46" s="3">
         <v>0.1</v>
       </c>
       <c r="J46" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>2.3000000000000003</v>
+        <v>7.7</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>33</v>
@@ -3143,33 +3101,33 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>110</v>
+        <v>235</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>111</v>
+        <v>236</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E47">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F47">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H47" s="2">
-        <v>5.3739996951159196E-3</v>
+        <v>6.5170950498219301E-3</v>
       </c>
       <c r="I47" s="3">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J47" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.2</v>
+        <v>4</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>33</v>
@@ -3177,33 +3135,35 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C48" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D48" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E48">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="F48">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H48" s="2">
-        <v>4.0930964868529799E-3</v>
+        <v>1.9298375811925401E-3</v>
       </c>
       <c r="I48" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="J48" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>1.1000000000000001</v>
+        <v>6.8000000000000007</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>33</v>
@@ -3211,33 +3171,35 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>220</v>
+        <v>54</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C49" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="D49" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E49">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F49">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H49" s="2">
-        <v>4.0131104964284299E-3</v>
+        <v>1.8554944377140699E-3</v>
       </c>
       <c r="I49" s="3">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="J49" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.4</v>
+        <v>1.56</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>33</v>
@@ -3245,33 +3207,33 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E50">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="F50">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H50" s="2">
-        <v>3.09635941517525E-3</v>
+        <v>6.5954579555748804E-3</v>
       </c>
       <c r="I50" s="3">
         <v>0.1</v>
       </c>
       <c r="J50" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>6.2</v>
+        <v>0.4</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>33</v>
@@ -3279,33 +3241,33 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>200</v>
+        <v>94</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>201</v>
+        <v>95</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E51">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="F51">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H51" s="2">
-        <v>2.75940391735065E-3</v>
+        <v>5.8288025643596902E-3</v>
       </c>
       <c r="I51" s="3">
         <v>0.1</v>
       </c>
       <c r="J51" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.4</v>
+        <v>2.3000000000000003</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>33</v>
@@ -3313,33 +3275,33 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>152</v>
+        <v>111</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H52" s="2">
-        <v>2.6052038183921001E-3</v>
+        <v>5.3739996951159196E-3</v>
       </c>
       <c r="I52" s="3">
         <v>0.1</v>
       </c>
       <c r="J52" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>33</v>
@@ -3347,33 +3309,33 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>155</v>
+        <v>90</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E53">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F53">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H53" s="2">
-        <v>2.10699478479152E-3</v>
+        <v>4.0930964868529799E-3</v>
       </c>
       <c r="I53" s="3">
         <v>0.1</v>
       </c>
       <c r="J53" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.30000000000000004</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>33</v>
@@ -3381,33 +3343,33 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E54">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F54">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H54" s="2">
-        <v>1.9790018792487998E-3</v>
+        <v>4.0131104964284299E-3</v>
       </c>
       <c r="I54" s="3">
         <v>0.1</v>
       </c>
       <c r="J54" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>33</v>
@@ -3415,33 +3377,33 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>100</v>
+        <v>36</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E55">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="F55">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H55" s="2">
-        <v>1.82315794138915E-3</v>
+        <v>3.09635941517525E-3</v>
       </c>
       <c r="I55" s="3">
         <v>0.1</v>
       </c>
       <c r="J55" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>3.2</v>
+        <v>6.2</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>33</v>
@@ -3449,33 +3411,33 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>139</v>
+        <v>200</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>140</v>
+        <v>201</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E56">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F56">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H56" s="2">
-        <v>1.6545210927024301E-3</v>
+        <v>2.75940391735065E-3</v>
       </c>
       <c r="I56" s="3">
         <v>0.1</v>
       </c>
       <c r="J56" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.60000000000000009</v>
+        <v>0.4</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>33</v>
@@ -3483,33 +3445,33 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>24</v>
+        <v>151</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>25</v>
+        <v>152</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E57">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="F57">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H57" s="2">
-        <v>1.61526603171404E-3</v>
+        <v>2.6052038183921001E-3</v>
       </c>
       <c r="I57" s="3">
         <v>0.1</v>
       </c>
       <c r="J57" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>2.4000000000000004</v>
+        <v>0.1</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>33</v>
@@ -3517,33 +3479,33 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>64</v>
+        <v>155</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>65</v>
+        <v>156</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E58">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="F58">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H58" s="2">
-        <v>1.4018555820005201E-3</v>
+        <v>2.10699478479152E-3</v>
       </c>
       <c r="I58" s="3">
         <v>0.1</v>
       </c>
       <c r="J58" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>3.7</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>33</v>
@@ -3551,31 +3513,33 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>273</v>
+        <v>245</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
       <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
+      <c r="D59" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E59">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F59">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H59" s="2">
-        <v>1.37869193326458E-3</v>
+        <v>1.9790018792487998E-3</v>
       </c>
       <c r="I59" s="3">
         <v>0.1</v>
       </c>
       <c r="J59" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>33</v>
@@ -3583,33 +3547,33 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E60">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F60">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H60" s="2">
-        <v>1.2217153626484999E-3</v>
+        <v>1.82315794138915E-3</v>
       </c>
       <c r="I60" s="3">
         <v>0.1</v>
       </c>
       <c r="J60" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.9</v>
+        <v>3.2</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>33</v>
@@ -3617,33 +3581,33 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E61">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F61">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H61" s="2">
-        <v>1.08825989463903E-3</v>
+        <v>1.6545210927024301E-3</v>
       </c>
       <c r="I61" s="3">
         <v>0.1</v>
       </c>
       <c r="J61" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.2</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>33</v>
@@ -3651,33 +3615,33 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E62">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F62">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H62" s="2">
-        <v>9.8826713501710202E-4</v>
+        <v>1.61526603171404E-3</v>
       </c>
       <c r="I62" s="3">
         <v>0.1</v>
       </c>
       <c r="J62" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.4</v>
+        <v>2.4000000000000004</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>33</v>
@@ -3685,33 +3649,33 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>141</v>
+        <v>64</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>142</v>
+        <v>65</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E63">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="F63">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H63" s="2">
-        <v>9.1571009960330198E-4</v>
+        <v>1.4018555820005201E-3</v>
       </c>
       <c r="I63" s="3">
         <v>0.1</v>
       </c>
       <c r="J63" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.4</v>
+        <v>3.7</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>33</v>
@@ -3719,33 +3683,31 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>153</v>
+        <v>273</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>154</v>
+        <v>274</v>
       </c>
       <c r="C64" s="1"/>
-      <c r="D64" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="D64" s="1"/>
       <c r="E64">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F64">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H64" s="2">
-        <v>8.0193057609872099E-4</v>
+        <v>1.37869193326458E-3</v>
       </c>
       <c r="I64" s="3">
         <v>0.1</v>
       </c>
       <c r="J64" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>33</v>
@@ -3753,33 +3715,33 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E65">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H65" s="2">
-        <v>7.9450180747740902E-4</v>
+        <v>1.2217153626484999E-3</v>
       </c>
       <c r="I65" s="3">
         <v>0.1</v>
       </c>
       <c r="J65" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>33</v>
@@ -3787,33 +3749,33 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E66">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F66">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H66" s="2">
-        <v>5.8351784184450196E-4</v>
+        <v>1.08825989463903E-3</v>
       </c>
       <c r="I66" s="3">
         <v>0.1</v>
       </c>
       <c r="J66" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.70000000000000007</v>
+        <v>0.2</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>33</v>
@@ -3821,33 +3783,33 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E67">
-        <v>115</v>
+        <v>4</v>
       </c>
       <c r="F67">
-        <v>115</v>
+        <v>4</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H67" s="2">
-        <v>4.8768737396479798E-4</v>
+        <v>9.8826713501710202E-4</v>
       </c>
       <c r="I67" s="3">
         <v>0.1</v>
       </c>
       <c r="J67" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>11.5</v>
+        <v>0.4</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>33</v>
@@ -3855,33 +3817,33 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E68">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F68">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H68" s="2">
-        <v>3.8154983332061701E-4</v>
+        <v>9.1571009960330198E-4</v>
       </c>
       <c r="I68" s="3">
         <v>0.1</v>
       </c>
       <c r="J68" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>1.4000000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>33</v>
@@ -3889,33 +3851,33 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E69">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="F69">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H69" s="2">
-        <v>3.4685786490544398E-4</v>
+        <v>8.0193057609872099E-4</v>
       </c>
       <c r="I69" s="3">
         <v>0.1</v>
       </c>
       <c r="J69" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>3.9000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>33</v>
@@ -3923,291 +3885,281 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E70">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F70">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H70" s="2">
-        <v>1.43381974550578E-4</v>
+        <v>7.9450180747740902E-4</v>
       </c>
       <c r="I70" s="3">
         <v>0.1</v>
       </c>
       <c r="J70" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>2.2000000000000002</v>
+        <v>1</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A71" s="6"/>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7"/>
-      <c r="G71" s="6"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="J71" s="5">
-        <f>SUBTOTAL(109,J41:J70)</f>
-        <v>65.459999999999994</v>
-      </c>
-      <c r="K71" s="6"/>
+      <c r="A71" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71">
+        <v>7</v>
+      </c>
+      <c r="F71">
+        <v>7</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H71" s="2">
+        <v>5.8351784184450196E-4</v>
+      </c>
+      <c r="I71" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J71" s="3">
+        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
+      <c r="A72" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="3"/>
-      <c r="K72" s="1"/>
+      <c r="D72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E72">
+        <v>115</v>
+      </c>
+      <c r="F72">
+        <v>115</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H72" s="2">
+        <v>4.8768737396479798E-4</v>
+      </c>
+      <c r="I72" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J72" s="3">
+        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
+        <v>11.5</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A73" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="B73" s="1"/>
+      <c r="A73" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="3"/>
-      <c r="J73" s="3"/>
-      <c r="K73" s="1"/>
+      <c r="D73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73">
+        <v>14</v>
+      </c>
+      <c r="F73">
+        <v>14</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H73" s="2">
+        <v>3.8154983332061701E-4</v>
+      </c>
+      <c r="I73" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J73" s="3">
+        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>209</v>
+        <v>98</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>210</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E74">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F74">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H74" s="2">
-        <v>2.5919999999999899</v>
+        <v>3.4685786490544398E-4</v>
       </c>
       <c r="I74" s="3">
-        <v>55</v>
+        <v>0.1</v>
       </c>
       <c r="J74" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>55</v>
+        <v>3.9000000000000004</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E75">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F75">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H75" s="2">
-        <v>0.22597580422031999</v>
+        <v>1.43381974550578E-4</v>
       </c>
       <c r="I75" s="3">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="J75" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>80</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E76">
-        <v>1</v>
-      </c>
-      <c r="F76">
-        <v>1</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H76" s="2">
-        <v>0.21693293905467101</v>
-      </c>
-      <c r="I76" s="3">
-        <v>5</v>
-      </c>
-      <c r="J76" s="3">
-        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>5</v>
-      </c>
-      <c r="K76" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A76" s="6"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="J76" s="5">
+        <f>SUBTOTAL(109,J46:J75)</f>
+        <v>65.459999999999994</v>
+      </c>
+      <c r="K76" s="6"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E77">
-        <v>8</v>
-      </c>
-      <c r="F77">
-        <v>8</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H77" s="2">
-        <v>8.3237387944534794E-3</v>
-      </c>
-      <c r="I77" s="3">
-        <v>3</v>
-      </c>
-      <c r="J77" s="3">
-        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>24</v>
-      </c>
-      <c r="K77" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="1"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E78">
-        <v>16</v>
-      </c>
-      <c r="F78">
-        <v>16</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H78" s="2">
-        <v>2.3637440042078298E-2</v>
-      </c>
-      <c r="I78" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="J78" s="3">
-        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>8</v>
-      </c>
-      <c r="K78" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A78" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="1"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>212</v>
+        <v>15</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>212</v>
+        <v>16</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>213</v>
+        <v>17</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E79">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F79">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>214</v>
+        <v>19</v>
       </c>
       <c r="H79" s="2">
-        <v>1.3933091100481101</v>
+        <v>0.22597580422031999</v>
       </c>
       <c r="I79" s="3">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="J79" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>20</v>
@@ -4215,12 +4167,14 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>247</v>
+        <v>102</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C80" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="D80" s="1" t="s">
         <v>18</v>
       </c>
@@ -4231,17 +4185,17 @@
         <v>1</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H80" s="2">
-        <v>8.3392972676616703E-2</v>
+        <v>0.21693293905467101</v>
       </c>
       <c r="I80" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J80" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K80" s="1" t="s">
         <v>20</v>
@@ -4249,469 +4203,466 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>97</v>
+        <v>310</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E81">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F81">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>319</v>
+        <v>19</v>
       </c>
       <c r="H81" s="2">
-        <v>1.7672573831909701E-2</v>
+        <v>8.3237387944534794E-3</v>
       </c>
       <c r="I81" s="3">
         <v>3</v>
       </c>
       <c r="J81" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="K81" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A82" s="6"/>
-      <c r="B82" s="6"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
-      <c r="G82" s="6"/>
-      <c r="H82" s="8"/>
-      <c r="I82" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="J82" s="5">
-        <f>SUBTOTAL(109,J74:J81)</f>
-        <v>275</v>
-      </c>
-      <c r="K82" s="6"/>
+      <c r="A82" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E82">
+        <v>16</v>
+      </c>
+      <c r="F82">
+        <v>16</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H82" s="2">
+        <v>2.3637440042078298E-2</v>
+      </c>
+      <c r="I82" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J82" s="3">
+        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
+        <v>8</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A83" s="6" t="s">
-        <v>349</v>
-      </c>
-      <c r="B83" s="1"/>
+      <c r="A83" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>248</v>
+      </c>
       <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="2"/>
-      <c r="I83" s="3"/>
-      <c r="J83" s="3"/>
-      <c r="K83" s="1"/>
+      <c r="D83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H83" s="2">
+        <v>8.3392972676616703E-2</v>
+      </c>
+      <c r="I83" s="3">
+        <v>10</v>
+      </c>
+      <c r="J83" s="3">
+        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
+        <v>10</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E84">
+        <v>21</v>
+      </c>
+      <c r="F84">
+        <v>21</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="H84" s="2">
+        <v>1.7672573831909701E-2</v>
+      </c>
+      <c r="I84" s="3">
+        <v>3</v>
+      </c>
+      <c r="J84" s="3">
+        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
+        <v>63</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" s="6"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="J85" s="5">
+        <f>SUBTOTAL(109,J79:J84)</f>
+        <v>190</v>
+      </c>
+      <c r="K85" s="6"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A86" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="1"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B87" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E84">
-        <v>1</v>
-      </c>
-      <c r="F84">
-        <v>1</v>
-      </c>
-      <c r="G84" s="1" t="s">
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="H84" s="2">
+      <c r="H87" s="2">
         <v>8.5092287144154594E-2</v>
       </c>
-      <c r="I84" s="3">
+      <c r="I87" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
         <v>2.1273071786038646</v>
       </c>
-      <c r="J84" s="3">
+      <c r="J87" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
         <v>2.1273071786038646</v>
       </c>
-      <c r="K84" s="1" t="s">
+      <c r="K87" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E85">
-        <v>1</v>
-      </c>
-      <c r="F85">
-        <v>1</v>
-      </c>
-      <c r="G85" s="1" t="s">
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="H85" s="2">
+      <c r="H88" s="2">
         <v>7.3665606655185803E-2</v>
       </c>
-      <c r="I85" s="3">
+      <c r="I88" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
         <v>1.8416401663796451</v>
       </c>
-      <c r="J85" s="3">
+      <c r="J88" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
         <v>1.8416401663796451</v>
       </c>
-      <c r="K85" s="1" t="s">
+      <c r="K88" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E86">
+      <c r="E89">
         <v>4</v>
       </c>
-      <c r="F86">
+      <c r="F89">
         <v>4</v>
       </c>
-      <c r="G86" s="1" t="s">
+      <c r="G89" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="H86" s="2">
+      <c r="H89" s="2">
         <v>6.4721681345502893E-2</v>
       </c>
-      <c r="I86" s="3">
+      <c r="I89" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
         <v>1.6180420336375723</v>
       </c>
-      <c r="J86" s="3">
+      <c r="J89" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
         <v>6.4721681345502891</v>
       </c>
-      <c r="K86" s="1" t="s">
+      <c r="K89" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1" t="s">
+      <c r="C90" s="1"/>
+      <c r="D90" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E87">
-        <v>1</v>
-      </c>
-      <c r="F87">
-        <v>1</v>
-      </c>
-      <c r="G87" s="1" t="s">
+      <c r="E90">
+        <v>1</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="H87" s="2">
+      <c r="H90" s="2">
         <v>5.05349943125072E-2</v>
       </c>
-      <c r="I87" s="3">
+      <c r="I90" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
         <v>1.26337485781268</v>
       </c>
-      <c r="J87" s="3">
+      <c r="J90" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
         <v>1.26337485781268</v>
       </c>
-      <c r="K87" s="1" t="s">
+      <c r="K90" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E88">
-        <v>1</v>
-      </c>
-      <c r="F88">
-        <v>1</v>
-      </c>
-      <c r="G88" s="1" t="s">
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="G91" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="H88" s="2">
+      <c r="H91" s="2">
         <v>4.67514374091186E-2</v>
       </c>
-      <c r="I88" s="3">
+      <c r="I91" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
         <v>1.168785935227965</v>
       </c>
-      <c r="J88" s="3">
+      <c r="J91" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
         <v>1.168785935227965</v>
       </c>
-      <c r="K88" s="1" t="s">
+      <c r="K91" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E89">
+      <c r="E92">
         <v>2</v>
       </c>
-      <c r="F89">
+      <c r="F92">
         <v>2</v>
       </c>
-      <c r="G89" s="1" t="s">
+      <c r="G92" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="H89" s="2">
+      <c r="H92" s="2">
         <v>3.6075401997775799E-2</v>
       </c>
-      <c r="I89" s="3">
+      <c r="I92" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
         <v>0.901885049944395</v>
       </c>
-      <c r="J89" s="3">
+      <c r="J92" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
         <v>1.80377009988879</v>
       </c>
-      <c r="K89" s="1" t="s">
+      <c r="K92" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="D90" s="1" t="s">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E90">
+      <c r="E93">
         <v>2</v>
       </c>
-      <c r="F90">
+      <c r="F93">
         <v>2</v>
       </c>
-      <c r="G90" s="1" t="s">
+      <c r="G93" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="H90" s="2">
+      <c r="H93" s="2">
         <v>3.0151351603941601E-2</v>
       </c>
-      <c r="I90" s="3">
+      <c r="I93" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
         <v>0.75378379009854002</v>
       </c>
-      <c r="J90" s="3">
+      <c r="J93" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
         <v>1.50756758019708</v>
       </c>
-      <c r="K90" s="1" t="s">
+      <c r="K93" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D91" s="1" t="s">
+      <c r="D94" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E91">
+      <c r="E94">
         <v>2</v>
       </c>
-      <c r="F91">
+      <c r="F94">
         <v>2</v>
       </c>
-      <c r="G91" s="1" t="s">
+      <c r="G94" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="H91" s="2">
+      <c r="H94" s="2">
         <v>2.8532628598633401E-2</v>
       </c>
-      <c r="I91" s="3">
+      <c r="I94" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
         <v>0.71331571496583501</v>
       </c>
-      <c r="J91" s="3">
+      <c r="J94" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
         <v>1.42663142993167</v>
-      </c>
-      <c r="K91" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E92">
-        <v>2</v>
-      </c>
-      <c r="F92">
-        <v>2</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="H92" s="2">
-        <v>2.3034170462874301E-2</v>
-      </c>
-      <c r="I92" s="3">
-        <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.57585426157185748</v>
-      </c>
-      <c r="J92" s="3">
-        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>1.151708523143715</v>
-      </c>
-      <c r="K92" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E93">
-        <v>1</v>
-      </c>
-      <c r="F93">
-        <v>1</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="H93" s="2">
-        <v>2.11136589526097E-2</v>
-      </c>
-      <c r="I93" s="3">
-        <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.52784147381524249</v>
-      </c>
-      <c r="J93" s="3">
-        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.52784147381524249</v>
-      </c>
-      <c r="K93" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E94">
-        <v>1</v>
-      </c>
-      <c r="F94">
-        <v>1</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="H94" s="2">
-        <v>2.11136589526097E-2</v>
-      </c>
-      <c r="I94" s="3">
-        <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.52784147381524249</v>
-      </c>
-      <c r="J94" s="3">
-        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.52784147381524249</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>138</v>
@@ -4719,10 +4670,10 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>61</v>
+        <v>218</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>61</v>
+        <v>218</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
@@ -4738,15 +4689,15 @@
         <v>306</v>
       </c>
       <c r="H95" s="2">
-        <v>1.7787926666685699E-2</v>
+        <v>2.3034170462874301E-2</v>
       </c>
       <c r="I95" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.44469816666714246</v>
+        <v>0.57585426157185748</v>
       </c>
       <c r="J95" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.88939633333428492</v>
+        <v>1.151708523143715</v>
       </c>
       <c r="K95" s="1" t="s">
         <v>138</v>
@@ -4754,34 +4705,36 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>87</v>
+        <v>352</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C96" s="1"/>
+        <v>352</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>353</v>
+      </c>
       <c r="D96" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E96">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F96">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H96" s="2">
-        <v>1.7407676226053399E-2</v>
+        <v>2.11136589526097E-2</v>
       </c>
       <c r="I96" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.43519190565133498</v>
+        <v>0.52784147381524249</v>
       </c>
       <c r="J96" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>3.0463433395593449</v>
+        <v>0.52784147381524249</v>
       </c>
       <c r="K96" s="1" t="s">
         <v>138</v>
@@ -4789,36 +4742,36 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>44</v>
+        <v>255</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>45</v>
+        <v>255</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>46</v>
+        <v>354</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H97" s="2">
-        <v>1.56961656179215E-2</v>
+        <v>2.11136589526097E-2</v>
       </c>
       <c r="I97" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.39240414044803751</v>
+        <v>0.52784147381524249</v>
       </c>
       <c r="J97" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.78480828089607502</v>
+        <v>0.52784147381524249</v>
       </c>
       <c r="K97" s="1" t="s">
         <v>138</v>
@@ -4826,14 +4779,12 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>165</v>
+        <v>61</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>166</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C98" s="1"/>
       <c r="D98" s="1" t="s">
         <v>41</v>
       </c>
@@ -4847,15 +4798,15 @@
         <v>306</v>
       </c>
       <c r="H98" s="2">
-        <v>1.4578930145396801E-2</v>
+        <v>1.7787926666685699E-2</v>
       </c>
       <c r="I98" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.36447325363492</v>
+        <v>0.44469816666714246</v>
       </c>
       <c r="J98" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.72894650726984</v>
+        <v>0.88939633333428492</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>138</v>
@@ -4863,36 +4814,34 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>167</v>
+        <v>87</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>168</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E99">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F99">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H99" s="2">
-        <v>1.11808654909509E-2</v>
+        <v>1.7407676226053399E-2</v>
       </c>
       <c r="I99" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.27952163727377249</v>
+        <v>0.43519190565133498</v>
       </c>
       <c r="J99" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.55904327454754499</v>
+        <v>3.0463433395593449</v>
       </c>
       <c r="K99" s="1" t="s">
         <v>138</v>
@@ -4900,34 +4849,36 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>226</v>
+        <v>44</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C100" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D100" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F100">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H100" s="2">
-        <v>1.03978677308904E-2</v>
+        <v>1.56961656179215E-2</v>
       </c>
       <c r="I100" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.25994669327226</v>
+        <v>0.39240414044803751</v>
       </c>
       <c r="J100" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.25994669327226</v>
+        <v>0.78480828089607502</v>
       </c>
       <c r="K100" s="1" t="s">
         <v>138</v>
@@ -4935,34 +4886,36 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>243</v>
+        <v>165</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C101" s="1"/>
+        <v>165</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="D101" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H101" s="2">
-        <v>1.03737111930468E-2</v>
+        <v>1.4578930145396801E-2</v>
       </c>
       <c r="I101" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.25934277982616999</v>
+        <v>0.36447325363492</v>
       </c>
       <c r="J101" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.25934277982616999</v>
+        <v>0.72894650726984</v>
       </c>
       <c r="K101" s="1" t="s">
         <v>138</v>
@@ -4970,36 +4923,36 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>120</v>
+        <v>168</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F102">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H102" s="2">
-        <v>9.9653504016373705E-3</v>
+        <v>1.11808654909509E-2</v>
       </c>
       <c r="I102" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.24913376004093427</v>
+        <v>0.27952163727377249</v>
       </c>
       <c r="J102" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.24913376004093427</v>
+        <v>0.55904327454754499</v>
       </c>
       <c r="K102" s="1" t="s">
         <v>138</v>
@@ -5007,14 +4960,12 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>108</v>
+        <v>226</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>109</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
         <v>41</v>
       </c>
@@ -5028,15 +4979,15 @@
         <v>306</v>
       </c>
       <c r="H103" s="2">
-        <v>9.4023566772491202E-3</v>
+        <v>1.03978677308904E-2</v>
       </c>
       <c r="I103" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.23505891693122802</v>
+        <v>0.25994669327226</v>
       </c>
       <c r="J103" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.23505891693122802</v>
+        <v>0.25994669327226</v>
       </c>
       <c r="K103" s="1" t="s">
         <v>138</v>
@@ -5044,34 +4995,34 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>197</v>
+        <v>243</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>197</v>
+        <v>243</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E104">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F104">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H104" s="2">
-        <v>7.6897970469752596E-3</v>
+        <v>1.03737111930468E-2</v>
       </c>
       <c r="I104" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.19224492617438149</v>
+        <v>0.25934277982616999</v>
       </c>
       <c r="J104" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.76897970469752597</v>
+        <v>0.25934277982616999</v>
       </c>
       <c r="K104" s="1" t="s">
         <v>138</v>
@@ -5079,13 +5030,17 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>294</v>
+        <v>119</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="E105">
         <v>1</v>
       </c>
@@ -5096,15 +5051,15 @@
         <v>306</v>
       </c>
       <c r="H105" s="2">
-        <v>7.0274905067941101E-3</v>
+        <v>9.9653504016373705E-3</v>
       </c>
       <c r="I105" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.17568726266985274</v>
+        <v>0.24913376004093427</v>
       </c>
       <c r="J105" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.17568726266985274</v>
+        <v>0.24913376004093427</v>
       </c>
       <c r="K105" s="1" t="s">
         <v>138</v>
@@ -5112,34 +5067,36 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>219</v>
+        <v>108</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C106" s="1"/>
+        <v>108</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="D106" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H106" s="2">
-        <v>4.5074712851086397E-3</v>
+        <v>9.4023566772491202E-3</v>
       </c>
       <c r="I106" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>0.11268678212771599</v>
+        <v>0.23505891693122802</v>
       </c>
       <c r="J106" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.22537356425543198</v>
+        <v>0.23505891693122802</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>138</v>
@@ -5147,34 +5104,34 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>276</v>
+        <v>197</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>276</v>
+        <v>197</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E107">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F107">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H107" s="2">
-        <v>3.7022690200368001E-3</v>
+        <v>7.6897970469752596E-3</v>
       </c>
       <c r="I107" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>9.2556725500920006E-2</v>
+        <v>0.19224492617438149</v>
       </c>
       <c r="J107" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.18511345100184001</v>
+        <v>0.76897970469752597</v>
       </c>
       <c r="K107" s="1" t="s">
         <v>138</v>
@@ -5182,17 +5139,13 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>158</v>
+        <v>294</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>294</v>
+      </c>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
       <c r="E108">
         <v>1</v>
       </c>
@@ -5203,15 +5156,15 @@
         <v>306</v>
       </c>
       <c r="H108" s="2">
-        <v>3.6819844288875801E-3</v>
+        <v>7.0274905067941101E-3</v>
       </c>
       <c r="I108" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>9.2049610722189507E-2</v>
+        <v>0.17568726266985274</v>
       </c>
       <c r="J108" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>9.2049610722189507E-2</v>
+        <v>0.17568726266985274</v>
       </c>
       <c r="K108" s="1" t="s">
         <v>138</v>
@@ -5219,36 +5172,34 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>131</v>
+        <v>219</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E109">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F109">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H109" s="2">
-        <v>3.2938735539807299E-3</v>
+        <v>4.5074712851086397E-3</v>
       </c>
       <c r="I109" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>8.2346838849518253E-2</v>
+        <v>0.11268678212771599</v>
       </c>
       <c r="J109" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>8.2346838849518253E-2</v>
+        <v>0.22537356425543198</v>
       </c>
       <c r="K109" s="1" t="s">
         <v>138</v>
@@ -5256,36 +5207,34 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>361</v>
+        <v>276</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>360</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E110">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F110">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G110" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H110" s="2">
-        <v>3.2364357266563399E-3</v>
+        <v>3.7022690200368001E-3</v>
       </c>
       <c r="I110" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>8.0910893166408496E-2</v>
+        <v>9.2556725500920006E-2</v>
       </c>
       <c r="J110" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>8.0910893166408496E-2</v>
+        <v>0.18511345100184001</v>
       </c>
       <c r="K110" s="1" t="s">
         <v>138</v>
@@ -5293,13 +5242,13 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>41</v>
@@ -5314,15 +5263,15 @@
         <v>306</v>
       </c>
       <c r="H111" s="2">
-        <v>2.82405496915382E-3</v>
+        <v>3.6819844288875801E-3</v>
       </c>
       <c r="I111" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>7.0601374228845507E-2</v>
+        <v>9.2049610722189507E-2</v>
       </c>
       <c r="J111" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>7.0601374228845507E-2</v>
+        <v>9.2049610722189507E-2</v>
       </c>
       <c r="K111" s="1" t="s">
         <v>138</v>
@@ -5330,36 +5279,36 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H112" s="2">
-        <v>2.6503524775281402E-3</v>
+        <v>3.2938735539807299E-3</v>
       </c>
       <c r="I112" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>6.6258811938203502E-2</v>
+        <v>8.2346838849518253E-2</v>
       </c>
       <c r="J112" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.132517623876407</v>
+        <v>8.2346838849518253E-2</v>
       </c>
       <c r="K112" s="1" t="s">
         <v>138</v>
@@ -5367,13 +5316,13 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>74</v>
+        <v>360</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>74</v>
+        <v>360</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>75</v>
+        <v>359</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>41</v>
@@ -5388,15 +5337,15 @@
         <v>306</v>
       </c>
       <c r="H113" s="2">
-        <v>2.3926150264109301E-3</v>
+        <v>3.2364357266563399E-3</v>
       </c>
       <c r="I113" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>5.9815375660273257E-2</v>
+        <v>8.0910893166408496E-2</v>
       </c>
       <c r="J113" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>5.9815375660273257E-2</v>
+        <v>8.0910893166408496E-2</v>
       </c>
       <c r="K113" s="1" t="s">
         <v>138</v>
@@ -5404,34 +5353,36 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>92</v>
+        <v>136</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C114" s="1"/>
+        <v>136</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="D114" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E114">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F114">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G114" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H114" s="2">
-        <v>2.1743596159829498E-3</v>
+        <v>2.82405496915382E-3</v>
       </c>
       <c r="I114" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>5.4358990399573745E-2</v>
+        <v>7.0601374228845507E-2</v>
       </c>
       <c r="J114" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>0.48923091359616372</v>
+        <v>7.0601374228845507E-2</v>
       </c>
       <c r="K114" s="1" t="s">
         <v>138</v>
@@ -5439,36 +5390,36 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>308</v>
+        <v>130</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E115">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F115">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H115" s="2">
-        <v>1.8929715575404201E-3</v>
+        <v>2.6503524775281402E-3</v>
       </c>
       <c r="I115" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>4.7324288938510504E-2</v>
+        <v>6.6258811938203502E-2</v>
       </c>
       <c r="J115" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>4.7324288938510504E-2</v>
+        <v>0.132517623876407</v>
       </c>
       <c r="K115" s="1" t="s">
         <v>138</v>
@@ -5476,36 +5427,36 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>362</v>
+        <v>74</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>127</v>
+        <v>75</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E116">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F116">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G116" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H116" s="2">
-        <v>1.7634907513691699E-3</v>
+        <v>2.3926150264109301E-3</v>
       </c>
       <c r="I116" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>4.408726878422925E-2</v>
+        <v>5.9815375660273257E-2</v>
       </c>
       <c r="J116" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>8.81745375684585E-2</v>
+        <v>5.9815375660273257E-2</v>
       </c>
       <c r="K116" s="1" t="s">
         <v>138</v>
@@ -5513,36 +5464,34 @@
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>244</v>
+        <v>92</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>354</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E117">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F117">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G117" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H117" s="2">
-        <v>1.4291735606598299E-3</v>
+        <v>2.1743596159829498E-3</v>
       </c>
       <c r="I117" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>3.5729339016495748E-2</v>
+        <v>5.4358990399573745E-2</v>
       </c>
       <c r="J117" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>3.5729339016495748E-2</v>
+        <v>0.48923091359616372</v>
       </c>
       <c r="K117" s="1" t="s">
         <v>138</v>
@@ -5550,13 +5499,13 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>227</v>
+        <v>160</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>227</v>
+        <v>161</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>355</v>
+        <v>308</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>41</v>
@@ -5571,15 +5520,15 @@
         <v>306</v>
       </c>
       <c r="H118" s="2">
-        <v>1.4219521125267401E-3</v>
+        <v>1.8929715575404201E-3</v>
       </c>
       <c r="I118" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>3.5548802813168502E-2</v>
+        <v>4.7324288938510504E-2</v>
       </c>
       <c r="J118" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>3.5548802813168502E-2</v>
+        <v>4.7324288938510504E-2</v>
       </c>
       <c r="K118" s="1" t="s">
         <v>138</v>
@@ -5587,69 +5536,180 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>237</v>
+        <v>361</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>237</v>
+        <v>126</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>238</v>
+        <v>127</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E119">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F119">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>306</v>
       </c>
       <c r="H119" s="2">
-        <v>3.51995167382192E-4</v>
+        <v>1.7634907513691699E-3</v>
       </c>
       <c r="I119" s="3">
         <f>Table1_2[[#This Row],[Mass]]*25</f>
-        <v>8.7998791845548003E-3</v>
+        <v>4.408726878422925E-2</v>
       </c>
       <c r="J119" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>8.7998791845548003E-3</v>
+        <v>8.81745375684585E-2</v>
       </c>
       <c r="K119" s="1" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B120" s="1"/>
-      <c r="D120" s="1"/>
-      <c r="G120" s="1"/>
-      <c r="H120" s="2"/>
-      <c r="I120" s="11" t="s">
-        <v>350</v>
-      </c>
-      <c r="J120" s="5">
-        <f>SUBTOTAL(109,J84:J119)</f>
+      <c r="A120" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E120">
+        <v>1</v>
+      </c>
+      <c r="F120">
+        <v>1</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="H120" s="2">
+        <v>1.4291735606598299E-3</v>
+      </c>
+      <c r="I120" s="3">
+        <f>Table1_2[[#This Row],[Mass]]*25</f>
+        <v>3.5729339016495748E-2</v>
+      </c>
+      <c r="J120" s="3">
+        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
+        <v>3.5729339016495748E-2</v>
+      </c>
+      <c r="K120" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E121">
+        <v>1</v>
+      </c>
+      <c r="F121">
+        <v>1</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="H121" s="2">
+        <v>1.4219521125267401E-3</v>
+      </c>
+      <c r="I121" s="3">
+        <f>Table1_2[[#This Row],[Mass]]*25</f>
+        <v>3.5548802813168502E-2</v>
+      </c>
+      <c r="J121" s="3">
+        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
+        <v>3.5548802813168502E-2</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E122">
+        <v>1</v>
+      </c>
+      <c r="F122">
+        <v>1</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="H122" s="2">
+        <v>3.51995167382192E-4</v>
+      </c>
+      <c r="I122" s="3">
+        <f>Table1_2[[#This Row],[Mass]]*25</f>
+        <v>8.7998791845548003E-3</v>
+      </c>
+      <c r="J122" s="3">
+        <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
+        <v>8.7998791845548003E-3</v>
+      </c>
+      <c r="K122" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B123" s="1"/>
+      <c r="D123" s="1"/>
+      <c r="G123" s="1"/>
+      <c r="H123" s="2"/>
+      <c r="I123" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="J123" s="5">
+        <f>SUBTOTAL(109,J87:J122)</f>
         <v>29.40886019928951</v>
       </c>
-      <c r="K120" s="1"/>
-    </row>
-    <row r="121" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="122" spans="1:11" s="7" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="I122" s="9" t="s">
+      <c r="K123" s="1"/>
+    </row>
+    <row r="124" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="125" spans="1:11" s="7" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="I125" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="J122" s="4">
-        <f>Table1_2[[#Totals],[Row Price]]+J82+J71+J39+J28+J12</f>
+      <c r="J125" s="4">
+        <f>Table1_2[[#Totals],[Row Price]]+J85+J76+J44+J26+J12+J33</f>
         <v>935.82910659187382</v>
       </c>
-      <c r="K122" s="5"/>
+      <c r="K125" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="58" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Cleaning up BOM part names
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 3D 400 BOM.xlsx
+++ b/BOM/V-King PRO 3D 400 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="555" documentId="11_C72AD000C5F844E0111E73BF19DBFC71502D2EF0" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{22BF3F69-38AC-4792-80AF-D4DF29FBDE48}"/>
+  <xr:revisionPtr revIDLastSave="611" documentId="11_C72AD000C5F844E0111E73BF19DBFC71502D2EF0" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{B8815D81-FE60-4407-BEC3-2FB86DC17D2A}"/>
   <bookViews>
-    <workbookView xWindow="2112" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3048" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$1:$K$122</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="423">
   <si>
     <t>Part Name</t>
   </si>
@@ -1000,9 +1000,6 @@
     <t>Controller Card</t>
   </si>
   <si>
-    <t>Bed Heater</t>
-  </si>
-  <si>
     <t>Leveling Probe</t>
   </si>
   <si>
@@ -1130,6 +1127,180 @@
   </si>
   <si>
     <t>Heatbed components</t>
+  </si>
+  <si>
+    <t>Filament Holder Rod</t>
+  </si>
+  <si>
+    <t>Filament Holder Nut</t>
+  </si>
+  <si>
+    <t>LCD Rear Cover</t>
+  </si>
+  <si>
+    <t>LCD Front Cover</t>
+  </si>
+  <si>
+    <t>12864 LCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAN 40-10mm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optical Sensor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssr-40 DA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E3d Hotend </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GT2 Motor Pulley 20T </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GT2 Pulley 20NT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GT2 Pulley 20T </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bearing 5-16-5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5 T-Nut Square </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5 Tee Nut </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5x35 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5x30 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5X25 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5x10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5x10 Hex </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4x20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4x16 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4x12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4x10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3X25 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3x20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5 Nut </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3x14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3x12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3x10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4 NUT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3x8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3 Lock Nut </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3 NUT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2028 L Bracket </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5x565 ROD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5 Thumb Screw 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y End Stop Buddy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filament Sensor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSR Heat Sink Fan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAN 60-10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5x20 Hex </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5x30 Hex </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5 Washer </t>
+  </si>
+  <si>
+    <t>M5 Washer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5 8OD Washer </t>
+  </si>
+  <si>
+    <t>M5 8OD Washer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4 Washer </t>
+  </si>
+  <si>
+    <t>M4 Washer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3 Washer </t>
+  </si>
+  <si>
+    <t>M3 Washer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5 Lock Nut </t>
+  </si>
+  <si>
+    <t>M5 Lock Nut</t>
+  </si>
+  <si>
+    <t>220AC 1000w 400*400</t>
+  </si>
+  <si>
+    <t>220VAC 1000W Silicone Pad</t>
+  </si>
+  <si>
+    <t>400*400*6 Build Plate</t>
+  </si>
+  <si>
+    <t>Aluminum Build Plate</t>
+  </si>
+  <si>
+    <t>Belt torque transfer rod</t>
   </si>
 </sst>
 </file>
@@ -1688,7 +1859,9 @@
   </sheetPr>
   <dimension ref="A1:K125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1749,10 +1922,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="3"/>
@@ -1761,13 +1934,13 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>41</v>
@@ -1835,13 +2008,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>41</v>
@@ -1914,7 +2087,9 @@
       <c r="B8" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>365</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>41</v>
       </c>
@@ -1949,7 +2124,9 @@
       <c r="B9" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>367</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1984,7 +2161,9 @@
       <c r="B10" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>368</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>41</v>
       </c>
@@ -2019,7 +2198,9 @@
       <c r="B11" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>366</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>41</v>
       </c>
@@ -2053,11 +2234,11 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J12" s="5">
         <f>SUBTOTAL(109,J4:J11)</f>
@@ -2080,10 +2261,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2131,7 +2312,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>146</v>
@@ -2167,7 +2348,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>262</v>
@@ -2203,13 +2384,13 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>18</v>
@@ -2239,13 +2420,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>279</v>
+        <v>369</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>280</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>18</v>
@@ -2275,7 +2456,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>184</v>
+        <v>403</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>185</v>
@@ -2311,13 +2492,13 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>297</v>
+        <v>404</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>298</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>18</v>
@@ -2347,13 +2528,13 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>299</v>
+        <v>405</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>300</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>18</v>
@@ -2383,13 +2564,13 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>269</v>
+        <v>370</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>18</v>
@@ -2419,13 +2600,13 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>18</v>
@@ -2455,13 +2636,13 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>76</v>
+        <v>371</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>18</v>
@@ -2497,11 +2678,11 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J26" s="5">
         <f>SUBTOTAL(109,J15:J25)</f>
@@ -2524,7 +2705,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B28" s="1"/>
       <c r="D28" s="1"/>
@@ -2572,13 +2753,13 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>290</v>
+        <v>372</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>291</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>18</v>
@@ -2608,13 +2789,13 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>322</v>
+        <v>205</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>205</v>
+        <v>419</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>206</v>
+        <v>418</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>18</v>
@@ -2644,10 +2825,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>209</v>
+        <v>421</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>209</v>
+        <v>420</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>210</v>
@@ -2685,11 +2866,11 @@
       <c r="D33" s="1"/>
       <c r="F33" s="7"/>
       <c r="G33" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J33" s="5">
         <f>SUBTOTAL(109,J29:J32)</f>
@@ -2699,7 +2880,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B34" s="1"/>
       <c r="D34" s="1"/>
@@ -2711,13 +2892,13 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>143</v>
+        <v>373</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>144</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>18</v>
@@ -2753,7 +2934,7 @@
         <v>174</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>18</v>
@@ -2927,13 +3108,13 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>57</v>
+        <v>374</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>18</v>
@@ -2963,7 +3144,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>113</v>
+        <v>375</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>309</v>
@@ -2999,7 +3180,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>66</v>
+        <v>376</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>67</v>
@@ -3040,11 +3221,11 @@
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
       <c r="G44" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H44" s="8"/>
       <c r="I44" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J44" s="5">
         <f>SUBTOTAL(109,J35:J43)</f>
@@ -3054,7 +3235,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3067,10 +3248,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>410</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>70</v>
+        <v>411</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
@@ -3101,7 +3282,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>235</v>
+        <v>377</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>236</v>
@@ -3135,7 +3316,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>30</v>
+        <v>378</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>31</v>
@@ -3171,7 +3352,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>54</v>
+        <v>379</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>55</v>
@@ -3207,7 +3388,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>62</v>
+        <v>380</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>63</v>
@@ -3241,7 +3422,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>94</v>
+        <v>381</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>95</v>
@@ -3275,7 +3456,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>110</v>
+        <v>407</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>111</v>
@@ -3309,7 +3490,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>90</v>
+        <v>406</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>91</v>
@@ -3343,7 +3524,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>220</v>
+        <v>382</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>221</v>
@@ -3377,7 +3558,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>36</v>
+        <v>383</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>37</v>
@@ -3411,7 +3592,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>200</v>
+        <v>384</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>201</v>
@@ -3445,7 +3626,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>151</v>
+        <v>385</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>152</v>
@@ -3479,7 +3660,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>155</v>
+        <v>386</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>156</v>
@@ -3513,7 +3694,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>245</v>
+        <v>387</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>246</v>
@@ -3547,7 +3728,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>100</v>
+        <v>388</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>101</v>
@@ -3581,7 +3762,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>139</v>
+        <v>389</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>140</v>
@@ -3615,7 +3796,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>25</v>
@@ -3649,10 +3830,10 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>64</v>
+        <v>416</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>65</v>
+        <v>417</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
@@ -3683,7 +3864,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>273</v>
+        <v>390</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>274</v>
@@ -3715,7 +3896,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>88</v>
+        <v>391</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>89</v>
@@ -3749,7 +3930,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>147</v>
+        <v>392</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>148</v>
@@ -3783,7 +3964,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>80</v>
+        <v>393</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>81</v>
@@ -3817,7 +3998,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>141</v>
+        <v>394</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>142</v>
@@ -3851,7 +4032,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>153</v>
+        <v>395</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>154</v>
@@ -3885,7 +4066,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>52</v>
+        <v>396</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>53</v>
@@ -3919,7 +4100,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>149</v>
+        <v>397</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>150</v>
@@ -3953,10 +4134,10 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>34</v>
+        <v>408</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>35</v>
+        <v>409</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
@@ -3987,7 +4168,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>78</v>
+        <v>398</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>79</v>
@@ -4021,10 +4202,10 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>98</v>
+        <v>412</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>99</v>
+        <v>413</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
@@ -4055,10 +4236,10 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>50</v>
+        <v>414</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>51</v>
+        <v>415</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
@@ -4097,7 +4278,7 @@
       <c r="G76" s="6"/>
       <c r="H76" s="2"/>
       <c r="I76" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J76" s="5">
         <f>SUBTOTAL(109,J46:J75)</f>
@@ -4118,7 +4299,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -4131,7 +4312,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>16</v>
@@ -4167,7 +4348,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>103</v>
@@ -4239,7 +4420,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>27</v>
+        <v>399</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>28</v>
@@ -4275,12 +4456,14 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>247</v>
+        <v>400</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C83" s="1"/>
+      <c r="C83" s="1" t="s">
+        <v>422</v>
+      </c>
       <c r="D83" s="1" t="s">
         <v>18</v>
       </c>
@@ -4309,7 +4492,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>97</v>
@@ -4353,7 +4536,7 @@
       <c r="G85" s="6"/>
       <c r="H85" s="8"/>
       <c r="I85" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J85" s="5">
         <f>SUBTOTAL(109,J79:J84)</f>
@@ -4363,7 +4546,7 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -4596,13 +4779,13 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>41</v>
@@ -4633,13 +4816,13 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>357</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>41</v>
@@ -4705,13 +4888,13 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>353</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>41</v>
@@ -4748,7 +4931,7 @@
         <v>255</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>41</v>
@@ -5316,13 +5499,13 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>41</v>
@@ -5464,7 +5647,7 @@
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>92</v>
+        <v>401</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>93</v>
@@ -5499,7 +5682,7 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>160</v>
+        <v>402</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>161</v>
@@ -5536,7 +5719,7 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>126</v>
@@ -5579,7 +5762,7 @@
         <v>244</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>41</v>
@@ -5616,7 +5799,7 @@
         <v>227</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>41</v>
@@ -5688,7 +5871,7 @@
       <c r="G123" s="1"/>
       <c r="H123" s="2"/>
       <c r="I123" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J123" s="5">
         <f>SUBTOTAL(109,J87:J122)</f>
@@ -5699,7 +5882,7 @@
     <row r="124" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="125" spans="1:11" s="7" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="I125" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J125" s="4">
         <f>Table1_2[[#Totals],[Row Price]]+J85+J76+J44+J26+J12+J33</f>

</xml_diff>

<commit_message>
updatet bom fastners only
M5x10+washers 8 of each
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 3D 400 BOM.xlsx
+++ b/BOM/V-King PRO 3D 400 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="611" documentId="11_C72AD000C5F844E0111E73BF19DBFC71502D2EF0" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{B8815D81-FE60-4407-BEC3-2FB86DC17D2A}"/>
+  <xr:revisionPtr revIDLastSave="612" documentId="11_C72AD000C5F844E0111E73BF19DBFC71502D2EF0" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{7CC4538E-5EF8-402E-BEAA-CEF2CC8AD8EE}"/>
   <bookViews>
-    <workbookView xWindow="3048" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3984" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -1859,8 +1859,8 @@
   </sheetPr>
   <dimension ref="A1:K125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3568,10 +3568,10 @@
         <v>18</v>
       </c>
       <c r="E55">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="F55">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>26</v>
@@ -3584,7 +3584,7 @@
       </c>
       <c r="J55" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>6.2</v>
+        <v>7.4</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>33</v>
@@ -4144,10 +4144,10 @@
         <v>18</v>
       </c>
       <c r="E72">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="F72">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>26</v>
@@ -4160,7 +4160,7 @@
       </c>
       <c r="J72" s="3">
         <f>Table1_2[[#This Row],[Item Price]]*Table1_2[[#This Row],[Order Quantity]]</f>
-        <v>11.5</v>
+        <v>12.3</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>33</v>
@@ -4282,7 +4282,7 @@
       </c>
       <c r="J76" s="5">
         <f>SUBTOTAL(109,J46:J75)</f>
-        <v>65.459999999999994</v>
+        <v>67.460000000000008</v>
       </c>
       <c r="K76" s="6"/>
     </row>
@@ -5886,7 +5886,7 @@
       </c>
       <c r="J125" s="4">
         <f>Table1_2[[#Totals],[Row Price]]+J85+J76+J44+J26+J12+J33</f>
-        <v>935.82910659187382</v>
+        <v>937.82910659187394</v>
       </c>
       <c r="K125" s="5"/>
     </row>

</xml_diff>

<commit_message>
Updated silicone heater link
link was wrong dimension - ask for more power
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 3D 400 BOM.xlsx
+++ b/BOM/V-King PRO 3D 400 BOM.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="339" documentId="8_{BF069A2D-0DEC-4E7D-97BD-1CEA86ABCA06}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{8FD7616E-84C9-4E23-9030-07FE6B24726B}"/>
+  <xr:revisionPtr revIDLastSave="340" documentId="8_{BF069A2D-0DEC-4E7D-97BD-1CEA86ABCA06}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{8B0B7831-817F-4499-B853-F44EE565E2F3}"/>
   <bookViews>
-    <workbookView xWindow="5856" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6792" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
     <sheet name="Hardware" sheetId="3" r:id="rId2"/>
-    <sheet name="Fastners" sheetId="1" r:id="rId3"/>
+    <sheet name="Fasteners" sheetId="1" r:id="rId3"/>
     <sheet name="Components" sheetId="5" r:id="rId4"/>
     <sheet name="PrintedParts" sheetId="2" r:id="rId5"/>
   </sheets>
@@ -1378,7 +1378,7 @@
         <v>168</v>
       </c>
       <c r="B6" s="12">
-        <f>Fastners!F29</f>
+        <f>Fasteners!F29</f>
         <v>85</v>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>